<commit_message>
Add code for envelope and keyboard modules
</commit_message>
<xml_diff>
--- a/Notes/KeyResistorChain.xlsx
+++ b/Notes/KeyResistorChain.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sondre\Documents\TinySynth\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4549DED6-7B58-42F3-B13A-1759B94ECFD3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04214307-DCCD-49AF-B13D-AE1406CB7FA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="870" yWindow="-110" windowWidth="31240" windowHeight="18220" xr2:uid="{CFF4FFF0-1F19-4673-97A5-F2735B33FE45}"/>
   </bookViews>
@@ -202,7 +202,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -281,7 +281,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2372,7 +2372,7 @@
   <dimension ref="B1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2431,7 +2431,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <f>$C$1*C4/(1-C4)</f>
+        <f t="shared" ref="D4:D23" si="0">$C$1*C4/(1-C4)</f>
         <v>0</v>
       </c>
       <c r="E4">
@@ -2444,7 +2444,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2">
-        <f>G4/(G4+$C$1)</f>
+        <f t="shared" ref="H4:H24" si="1">G4/(G4+$C$1)</f>
         <v>0</v>
       </c>
       <c r="I4" s="6">
@@ -2465,7 +2465,7 @@
         <v>0.05</v>
       </c>
       <c r="D5" s="3">
-        <f>$C$1*C5/(1-C5)</f>
+        <f t="shared" si="0"/>
         <v>526.31578947368428</v>
       </c>
       <c r="E5" s="3">
@@ -2480,11 +2480,11 @@
         <v>680</v>
       </c>
       <c r="H5" s="2">
-        <f>G5/(G5+$C$1)</f>
+        <f t="shared" si="1"/>
         <v>6.3670411985018729E-2</v>
       </c>
       <c r="I5" s="6">
-        <f t="shared" ref="I5:I24" si="0">ROUND(255*H5,0)</f>
+        <f t="shared" ref="I5:I24" si="2">ROUND(255*H5,0)</f>
         <v>16</v>
       </c>
       <c r="J5" s="6">
@@ -2504,11 +2504,11 @@
         <v>0.1</v>
       </c>
       <c r="D6" s="3">
-        <f>$C$1*C6/(1-C6)</f>
+        <f t="shared" si="0"/>
         <v>1111.1111111111111</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" ref="E6:E17" si="1">D6-D5</f>
+        <f t="shared" ref="E6:E17" si="3">D6-D5</f>
         <v>584.79532163742681</v>
       </c>
       <c r="F6">
@@ -2516,19 +2516,19 @@
         <v>680</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6:G17" si="2">G5+F6</f>
+        <f t="shared" ref="G6:G17" si="4">G5+F6</f>
         <v>1360</v>
       </c>
       <c r="H6" s="2">
-        <f>G6/(G6+$C$1)</f>
+        <f t="shared" si="1"/>
         <v>0.11971830985915492</v>
       </c>
       <c r="I6" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="J6" s="6">
-        <f t="shared" ref="J6:J17" si="3">I6-I5</f>
+        <f t="shared" ref="J6:J17" si="5">I6-I5</f>
         <v>15</v>
       </c>
       <c r="L6">
@@ -2544,11 +2544,11 @@
         <v>0.15</v>
       </c>
       <c r="D7" s="3">
-        <f>$C$1*C7/(1-C7)</f>
+        <f t="shared" si="0"/>
         <v>1764.7058823529412</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>653.59477124183013</v>
       </c>
       <c r="F7">
@@ -2556,19 +2556,19 @@
         <v>680</v>
       </c>
       <c r="G7">
+        <f t="shared" si="4"/>
+        <v>2040</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16943521594684385</v>
+      </c>
+      <c r="I7" s="6">
         <f t="shared" si="2"/>
-        <v>2040</v>
-      </c>
-      <c r="H7" s="2">
-        <f>G7/(G7+$C$1)</f>
-        <v>0.16943521594684385</v>
-      </c>
-      <c r="I7" s="6">
-        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="J7" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="L7">
@@ -2584,11 +2584,11 @@
         <v>0.2</v>
       </c>
       <c r="D8" s="3">
-        <f>$C$1*C8/(1-C8)</f>
+        <f t="shared" si="0"/>
         <v>2500</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>735.29411764705878</v>
       </c>
       <c r="F8">
@@ -2596,19 +2596,19 @@
         <v>680</v>
       </c>
       <c r="G8">
+        <f t="shared" si="4"/>
+        <v>2720</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.21383647798742139</v>
+      </c>
+      <c r="I8" s="6">
         <f t="shared" si="2"/>
-        <v>2720</v>
-      </c>
-      <c r="H8" s="2">
-        <f>G8/(G8+$C$1)</f>
-        <v>0.21383647798742139</v>
-      </c>
-      <c r="I8" s="6">
-        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="J8" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="L8">
@@ -2624,11 +2624,11 @@
         <v>0.25</v>
       </c>
       <c r="D9" s="3">
-        <f>$C$1*C9/(1-C9)</f>
+        <f t="shared" si="0"/>
         <v>3333.3333333333335</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>833.33333333333348</v>
       </c>
       <c r="F9">
@@ -2636,19 +2636,19 @@
         <v>1000</v>
       </c>
       <c r="G9">
+        <f t="shared" si="4"/>
+        <v>3720</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27113702623906705</v>
+      </c>
+      <c r="I9" s="6">
         <f t="shared" si="2"/>
-        <v>3720</v>
-      </c>
-      <c r="H9" s="2">
-        <f>G9/(G9+$C$1)</f>
-        <v>0.27113702623906705</v>
-      </c>
-      <c r="I9" s="6">
-        <f t="shared" si="0"/>
         <v>69</v>
       </c>
       <c r="J9" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="L9">
@@ -2664,11 +2664,11 @@
         <v>0.3</v>
       </c>
       <c r="D10" s="3">
-        <f>$C$1*C10/(1-C10)</f>
+        <f t="shared" si="0"/>
         <v>4285.7142857142862</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>952.38095238095275</v>
       </c>
       <c r="F10">
@@ -2676,19 +2676,19 @@
         <v>1000</v>
       </c>
       <c r="G10">
+        <f t="shared" si="4"/>
+        <v>4720</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.32065217391304346</v>
+      </c>
+      <c r="I10" s="6">
         <f t="shared" si="2"/>
-        <v>4720</v>
-      </c>
-      <c r="H10" s="2">
-        <f>G10/(G10+$C$1)</f>
-        <v>0.32065217391304346</v>
-      </c>
-      <c r="I10" s="6">
-        <f t="shared" si="0"/>
         <v>82</v>
       </c>
       <c r="J10" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="L10">
@@ -2705,11 +2705,11 @@
         <v>0.35</v>
       </c>
       <c r="D11" s="3">
-        <f>$C$1*C11/(1-C11)</f>
+        <f t="shared" si="0"/>
         <v>5384.6153846153848</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1098.9010989010985</v>
       </c>
       <c r="F11">
@@ -2717,19 +2717,19 @@
         <v>1000</v>
       </c>
       <c r="G11">
+        <f t="shared" si="4"/>
+        <v>5720</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.36386768447837148</v>
+      </c>
+      <c r="I11" s="6">
         <f t="shared" si="2"/>
-        <v>5720</v>
-      </c>
-      <c r="H11" s="2">
-        <f>G11/(G11+$C$1)</f>
-        <v>0.36386768447837148</v>
-      </c>
-      <c r="I11" s="6">
-        <f t="shared" si="0"/>
         <v>93</v>
       </c>
       <c r="J11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="L11" s="5"/>
@@ -2742,11 +2742,11 @@
         <v>0.4</v>
       </c>
       <c r="D12" s="3">
-        <f>$C$1*C12/(1-C12)</f>
+        <f t="shared" si="0"/>
         <v>6666.666666666667</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1282.0512820512822</v>
       </c>
       <c r="F12">
@@ -2754,19 +2754,19 @@
         <v>1500</v>
       </c>
       <c r="G12">
+        <f t="shared" si="4"/>
+        <v>7220</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.41927990708478513</v>
+      </c>
+      <c r="I12" s="6">
         <f t="shared" si="2"/>
-        <v>7220</v>
-      </c>
-      <c r="H12" s="2">
-        <f>G12/(G12+$C$1)</f>
-        <v>0.41927990708478513</v>
-      </c>
-      <c r="I12" s="6">
-        <f t="shared" si="0"/>
         <v>107</v>
       </c>
       <c r="J12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
     </row>
@@ -2778,11 +2778,11 @@
         <v>0.45</v>
       </c>
       <c r="D13" s="3">
-        <f>$C$1*C13/(1-C13)</f>
+        <f t="shared" si="0"/>
         <v>8181.8181818181811</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1515.1515151515141</v>
       </c>
       <c r="F13">
@@ -2790,19 +2790,19 @@
         <v>1500</v>
       </c>
       <c r="G13">
+        <f t="shared" si="4"/>
+        <v>8720</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.46581196581196582</v>
+      </c>
+      <c r="I13" s="6">
         <f t="shared" si="2"/>
-        <v>8720</v>
-      </c>
-      <c r="H13" s="2">
-        <f>G13/(G13+$C$1)</f>
-        <v>0.46581196581196582</v>
-      </c>
-      <c r="I13" s="6">
-        <f t="shared" si="0"/>
         <v>119</v>
       </c>
       <c r="J13" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
     </row>
@@ -2814,11 +2814,11 @@
         <v>0.5</v>
       </c>
       <c r="D14" s="3">
-        <f>$C$1*C14/(1-C14)</f>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1818.1818181818189</v>
       </c>
       <c r="F14">
@@ -2826,19 +2826,19 @@
         <v>2200</v>
       </c>
       <c r="G14">
+        <f t="shared" si="4"/>
+        <v>10920</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.52198852772466542</v>
+      </c>
+      <c r="I14" s="6">
         <f t="shared" si="2"/>
-        <v>10920</v>
-      </c>
-      <c r="H14" s="2">
-        <f>G14/(G14+$C$1)</f>
-        <v>0.52198852772466542</v>
-      </c>
-      <c r="I14" s="6">
-        <f t="shared" si="0"/>
         <v>133</v>
       </c>
       <c r="J14" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
     </row>
@@ -2850,11 +2850,11 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="D15" s="3">
-        <f>$C$1*C15/(1-C15)</f>
+        <f t="shared" si="0"/>
         <v>12222.222222222223</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2222.2222222222226</v>
       </c>
       <c r="F15">
@@ -2862,19 +2862,19 @@
         <v>2200</v>
       </c>
       <c r="G15">
+        <f t="shared" si="4"/>
+        <v>13120</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>0.56747404844290661</v>
+      </c>
+      <c r="I15" s="6">
         <f t="shared" si="2"/>
-        <v>13120</v>
-      </c>
-      <c r="H15" s="2">
-        <f>G15/(G15+$C$1)</f>
-        <v>0.56747404844290661</v>
-      </c>
-      <c r="I15" s="6">
-        <f t="shared" si="0"/>
         <v>145</v>
       </c>
       <c r="J15" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
     </row>
@@ -2886,11 +2886,11 @@
         <v>0.6</v>
       </c>
       <c r="D16" s="3">
-        <f>$C$1*C16/(1-C16)</f>
+        <f t="shared" si="0"/>
         <v>15000</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2777.7777777777774</v>
       </c>
       <c r="F16">
@@ -2898,19 +2898,19 @@
         <v>3300</v>
       </c>
       <c r="G16">
+        <f t="shared" si="4"/>
+        <v>16420</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>0.62149886449659353</v>
+      </c>
+      <c r="I16" s="6">
         <f t="shared" si="2"/>
-        <v>16420</v>
-      </c>
-      <c r="H16" s="2">
-        <f>G16/(G16+$C$1)</f>
-        <v>0.62149886449659353</v>
-      </c>
-      <c r="I16" s="6">
-        <f t="shared" si="0"/>
         <v>158</v>
       </c>
       <c r="J16" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
     </row>
@@ -2922,11 +2922,11 @@
         <v>0.65</v>
       </c>
       <c r="D17" s="3">
-        <f>$C$1*C17/(1-C17)</f>
+        <f t="shared" si="0"/>
         <v>18571.428571428572</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3571.4285714285725</v>
       </c>
       <c r="F17">
@@ -2934,19 +2934,19 @@
         <v>3300</v>
       </c>
       <c r="G17">
+        <f t="shared" si="4"/>
+        <v>19720</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>0.6635262449528937</v>
+      </c>
+      <c r="I17" s="6">
         <f t="shared" si="2"/>
-        <v>19720</v>
-      </c>
-      <c r="H17" s="2">
-        <f>G17/(G17+$C$1)</f>
-        <v>0.6635262449528937</v>
-      </c>
-      <c r="I17" s="6">
-        <f t="shared" si="0"/>
         <v>169</v>
       </c>
       <c r="J17" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
     </row>
@@ -2958,30 +2958,30 @@
         <v>0.7</v>
       </c>
       <c r="D18" s="3">
-        <f>$C$1*C18/(1-C18)</f>
+        <f t="shared" si="0"/>
         <v>23333.333333333328</v>
       </c>
       <c r="E18" s="3">
-        <f>D18-D17</f>
+        <f t="shared" ref="E18:E23" si="6">D18-D17</f>
         <v>4761.904761904756</v>
       </c>
       <c r="F18">
         <v>6800</v>
       </c>
       <c r="G18">
-        <f>G17+F18</f>
+        <f t="shared" ref="G18:G23" si="7">G17+F18</f>
         <v>26520</v>
       </c>
       <c r="H18" s="2">
-        <f>G18/(G18+$C$1)</f>
+        <f t="shared" si="1"/>
         <v>0.7261774370208105</v>
       </c>
       <c r="I18" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>185</v>
       </c>
       <c r="J18" s="6">
-        <f>I18-I17</f>
+        <f t="shared" ref="J18:J24" si="8">I18-I17</f>
         <v>16</v>
       </c>
     </row>
@@ -2993,11 +2993,11 @@
         <v>0.75</v>
       </c>
       <c r="D19" s="3">
-        <f>$C$1*C19/(1-C19)</f>
+        <f t="shared" si="0"/>
         <v>30000</v>
       </c>
       <c r="E19" s="3">
-        <f>D19-D18</f>
+        <f t="shared" si="6"/>
         <v>6666.6666666666715</v>
       </c>
       <c r="F19">
@@ -3005,19 +3005,19 @@
         <v>6800</v>
       </c>
       <c r="G19">
-        <f>G18+F19</f>
+        <f t="shared" si="7"/>
         <v>33320</v>
       </c>
       <c r="H19" s="2">
-        <f>G19/(G19+$C$1)</f>
+        <f t="shared" si="1"/>
         <v>0.76915974145891042</v>
       </c>
       <c r="I19" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>196</v>
       </c>
       <c r="J19" s="6">
-        <f>I19-I18</f>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
     </row>
@@ -3029,11 +3029,11 @@
         <v>0.8</v>
       </c>
       <c r="D20" s="3">
-        <f>$C$1*C20/(1-C20)</f>
+        <f t="shared" si="0"/>
         <v>40000.000000000007</v>
       </c>
       <c r="E20" s="3">
-        <f>D20-D19</f>
+        <f t="shared" si="6"/>
         <v>10000.000000000007</v>
       </c>
       <c r="F20">
@@ -3041,19 +3041,19 @@
         <v>10000</v>
       </c>
       <c r="G20">
-        <f>G19+F20</f>
+        <f t="shared" si="7"/>
         <v>43320</v>
       </c>
       <c r="H20" s="2">
-        <f>G20/(G20+$C$1)</f>
+        <f t="shared" si="1"/>
         <v>0.81245311327831959</v>
       </c>
       <c r="I20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>207</v>
       </c>
       <c r="J20" s="6">
-        <f>I20-I19</f>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
     </row>
@@ -3065,11 +3065,11 @@
         <v>0.85</v>
       </c>
       <c r="D21" s="3">
-        <f>$C$1*C21/(1-C21)</f>
+        <f t="shared" si="0"/>
         <v>56666.666666666657</v>
       </c>
       <c r="E21" s="3">
-        <f>D21-D20</f>
+        <f t="shared" si="6"/>
         <v>16666.66666666665</v>
       </c>
       <c r="F21">
@@ -3077,19 +3077,19 @@
         <v>15000</v>
       </c>
       <c r="G21">
-        <f>G20+F21</f>
+        <f t="shared" si="7"/>
         <v>58320</v>
       </c>
       <c r="H21" s="2">
-        <f>G21/(G21+$C$1)</f>
+        <f t="shared" si="1"/>
         <v>0.8536299765807962</v>
       </c>
       <c r="I21" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>218</v>
       </c>
       <c r="J21" s="6">
-        <f>I21-I20</f>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
     </row>
@@ -3101,11 +3101,11 @@
         <v>0.9</v>
       </c>
       <c r="D22" s="3">
-        <f>$C$1*C22/(1-C22)</f>
+        <f t="shared" si="0"/>
         <v>90000.000000000015</v>
       </c>
       <c r="E22" s="3">
-        <f>D22-D21</f>
+        <f t="shared" si="6"/>
         <v>33333.333333333358</v>
       </c>
       <c r="F22">
@@ -3113,19 +3113,19 @@
         <v>33000</v>
       </c>
       <c r="G22">
-        <f>G21+F22</f>
+        <f t="shared" si="7"/>
         <v>91320</v>
       </c>
       <c r="H22" s="2">
-        <f>G22/(G22+$C$1)</f>
+        <f t="shared" si="1"/>
         <v>0.90130280300039478</v>
       </c>
       <c r="I22" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>230</v>
       </c>
       <c r="J22" s="6">
-        <f>I22-I21</f>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
     </row>
@@ -3137,11 +3137,11 @@
         <v>0.95</v>
       </c>
       <c r="D23" s="3">
-        <f>$C$1*C23/(1-C23)</f>
+        <f t="shared" si="0"/>
         <v>189999.99999999983</v>
       </c>
       <c r="E23" s="3">
-        <f>D23-D22</f>
+        <f t="shared" si="6"/>
         <v>99999.999999999811</v>
       </c>
       <c r="F23">
@@ -3149,19 +3149,19 @@
         <v>100000</v>
       </c>
       <c r="G23">
-        <f>G22+F23</f>
+        <f t="shared" si="7"/>
         <v>191320</v>
       </c>
       <c r="H23" s="2">
-        <f>G23/(G23+$C$1)</f>
+        <f t="shared" si="1"/>
         <v>0.9503278362805484</v>
       </c>
       <c r="I23" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>242</v>
       </c>
       <c r="J23" s="6">
-        <f>I23-I22</f>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
     </row>
@@ -3185,15 +3185,15 @@
         <v>9.9999999999999997E+98</v>
       </c>
       <c r="H24" s="2">
-        <f>G24/(G24+$C$1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I24" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>255</v>
       </c>
       <c r="J24" s="6">
-        <f>I24-I23</f>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add config panel module
</commit_message>
<xml_diff>
--- a/Notes/KeyResistorChain.xlsx
+++ b/Notes/KeyResistorChain.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sondre\Documents\TinySynth\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sondre\Documents\Repositories\TinySynth\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAE0372-7E5E-4536-9C5B-4E8AFEAB8FA8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA50FED-E61A-4DC0-B0E9-C2649355C510}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10990" yWindow="1990" windowWidth="16280" windowHeight="14660" xr2:uid="{CFF4FFF0-1F19-4673-97A5-F2735B33FE45}"/>
+    <workbookView xWindow="-23190" yWindow="1935" windowWidth="21600" windowHeight="11835" xr2:uid="{CFF4FFF0-1F19-4673-97A5-F2735B33FE45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -278,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -288,6 +288,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6416,16 +6417,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>415925</xdr:colOff>
-      <xdr:row>289</xdr:row>
-      <xdr:rowOff>73025</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>273050</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>212725</xdr:colOff>
-      <xdr:row>304</xdr:row>
-      <xdr:rowOff>53975</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6752,19 +6753,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1B93E0-F104-4A6F-BDD7-A40B438CE94B}">
   <dimension ref="B1:Q326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A281" workbookViewId="0">
-      <selection activeCell="I312" sqref="I312"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="5" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.54296875" customWidth="1"/>
+    <col min="4" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
         <v>14</v>
       </c>
@@ -6772,7 +6773,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>30</v>
       </c>
@@ -6807,7 +6808,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -6848,7 +6849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -6894,7 +6895,7 @@
         <v>6.3314037626628072E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>25</v>
       </c>
@@ -6941,7 +6942,7 @@
         <v>0.11903039073806078</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -6988,7 +6989,7 @@
         <v>0.16859623733719248</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>26</v>
       </c>
@@ -7035,7 +7036,7 @@
         <v>0.21273516642547033</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -7082,7 +7083,7 @@
         <v>0.374095513748191</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>22</v>
       </c>
@@ -7130,7 +7131,7 @@
         <v>0.48046309696092621</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -7174,7 +7175,7 @@
         <v>0.55607814761215635</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -7217,7 +7218,7 @@
         <v>0.58357452966714907</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>27</v>
       </c>
@@ -7260,7 +7261,7 @@
         <v>0.6078147612156295</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -7303,7 +7304,7 @@
         <v>0.63892908827785821</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -7346,7 +7347,7 @@
         <v>0.66534008683068013</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -7389,7 +7390,7 @@
         <v>0.6761939218523878</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -7432,7 +7433,7 @@
         <v>0.68632416787264838</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>28</v>
       </c>
@@ -7474,7 +7475,7 @@
         <v>0.74131693198263382</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>2</v>
       </c>
@@ -7517,7 +7518,7 @@
         <v>0.77966714905933432</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>29</v>
       </c>
@@ -7560,7 +7561,7 @@
         <v>0.81946454413892911</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -7603,7 +7604,7 @@
         <v>0.8578147612156295</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>24</v>
       </c>
@@ -7646,7 +7647,7 @@
         <v>0.90303907380607817</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>0</v>
       </c>
@@ -7689,7 +7690,7 @@
         <v>0.95043415340086834</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>31</v>
       </c>
@@ -7728,7 +7729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -7741,7 +7742,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -7754,7 +7755,7 @@
         <v>1.6181535936466533</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -7767,7 +7768,7 @@
         <v>5.4886131999198904</v>
       </c>
     </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C47">
         <f>I4</f>
         <v>0</v>
@@ -7781,7 +7782,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="9">
+        <f>AVERAGE(C47:C48)</f>
+        <v>8</v>
+      </c>
       <c r="C48">
         <f t="shared" ref="C48:C65" si="10">I5</f>
         <v>16</v>
@@ -7795,7 +7800,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="9">
+        <f t="shared" ref="B49:B67" si="13">AVERAGE(C48:C49)</f>
+        <v>23.5</v>
+      </c>
       <c r="C49">
         <f t="shared" si="10"/>
         <v>31</v>
@@ -7809,7 +7818,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="9">
+        <f t="shared" si="13"/>
+        <v>37</v>
+      </c>
       <c r="C50">
         <f t="shared" si="10"/>
         <v>43</v>
@@ -7823,7 +7836,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="9">
+        <f t="shared" si="13"/>
+        <v>49</v>
+      </c>
       <c r="C51">
         <f t="shared" si="10"/>
         <v>55</v>
@@ -7837,7 +7854,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="9">
+        <f t="shared" si="13"/>
+        <v>62</v>
+      </c>
       <c r="C52">
         <f t="shared" si="10"/>
         <v>69</v>
@@ -7851,7 +7872,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="9">
+        <f t="shared" si="13"/>
+        <v>75.5</v>
+      </c>
       <c r="C53">
         <f t="shared" si="10"/>
         <v>82</v>
@@ -7865,7 +7890,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="9">
+        <f t="shared" si="13"/>
+        <v>87.5</v>
+      </c>
       <c r="C54">
         <f t="shared" si="10"/>
         <v>93</v>
@@ -7879,7 +7908,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="9">
+        <f t="shared" si="13"/>
+        <v>100</v>
+      </c>
       <c r="C55">
         <f t="shared" si="10"/>
         <v>107</v>
@@ -7893,7 +7926,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="9">
+        <f t="shared" si="13"/>
+        <v>113</v>
+      </c>
       <c r="C56">
         <f t="shared" si="10"/>
         <v>119</v>
@@ -7907,7 +7944,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="9">
+        <f t="shared" si="13"/>
+        <v>126</v>
+      </c>
       <c r="C57">
         <f t="shared" si="10"/>
         <v>133</v>
@@ -7921,7 +7962,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="9">
+        <f t="shared" si="13"/>
+        <v>139</v>
+      </c>
       <c r="C58">
         <f t="shared" si="10"/>
         <v>145</v>
@@ -7935,7 +7980,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="9">
+        <f t="shared" si="13"/>
+        <v>151.5</v>
+      </c>
       <c r="C59">
         <f t="shared" si="10"/>
         <v>158</v>
@@ -7949,7 +7998,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="9">
+        <f t="shared" si="13"/>
+        <v>163.5</v>
+      </c>
       <c r="C60">
         <f t="shared" si="10"/>
         <v>169</v>
@@ -7963,7 +8016,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="9">
+        <f t="shared" si="13"/>
+        <v>177</v>
+      </c>
       <c r="C61">
         <f t="shared" si="10"/>
         <v>185</v>
@@ -7977,7 +8034,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="9">
+        <f t="shared" si="13"/>
+        <v>190.5</v>
+      </c>
       <c r="C62">
         <f t="shared" si="10"/>
         <v>196</v>
@@ -7991,7 +8052,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="9">
+        <f t="shared" si="13"/>
+        <v>201.5</v>
+      </c>
       <c r="C63">
         <f t="shared" si="10"/>
         <v>207</v>
@@ -8005,7 +8070,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="9">
+        <f t="shared" si="13"/>
+        <v>212.5</v>
+      </c>
       <c r="C64">
         <f t="shared" si="10"/>
         <v>218</v>
@@ -8019,7 +8088,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="9">
+        <f t="shared" si="13"/>
+        <v>224</v>
+      </c>
       <c r="C65">
         <f t="shared" si="10"/>
         <v>230</v>
@@ -8033,7 +8106,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="9">
+        <f t="shared" si="13"/>
+        <v>236</v>
+      </c>
       <c r="C66">
         <f>I23</f>
         <v>242</v>
@@ -8047,7 +8124,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="9">
+        <f t="shared" si="13"/>
+        <v>248.5</v>
+      </c>
       <c r="C67">
         <f>I24</f>
         <v>255</v>
@@ -8061,7 +8142,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="71" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C71">
         <v>0</v>
       </c>
@@ -8074,3318 +8155,3318 @@
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C72">
         <v>1</v>
       </c>
       <c r="D72">
-        <f t="shared" ref="D72:D135" si="13">FLOOR((20*C72+128)/256,1)</f>
+        <f t="shared" ref="D72:D135" si="14">FLOOR((20*C72+128)/256,1)</f>
         <v>0</v>
       </c>
       <c r="E72">
-        <f t="shared" ref="E72:E135" si="14">19-D72</f>
+        <f t="shared" ref="E72:E135" si="15">19-D72</f>
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C73">
         <v>2</v>
       </c>
       <c r="D73">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="E73">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>19</v>
       </c>
     </row>
-    <row r="74" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C74">
         <v>3</v>
       </c>
       <c r="D74">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="E74">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>19</v>
       </c>
     </row>
-    <row r="75" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C75">
         <v>4</v>
       </c>
       <c r="D75">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="E75">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>19</v>
       </c>
     </row>
-    <row r="76" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C76">
         <v>5</v>
       </c>
       <c r="D76">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="E76">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C77">
         <v>6</v>
       </c>
       <c r="D77">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="E77">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C78">
         <v>7</v>
       </c>
       <c r="D78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E78">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C79">
         <v>8</v>
       </c>
       <c r="D79">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E79">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C80">
         <v>9</v>
       </c>
       <c r="D80">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E80">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C81">
         <v>10</v>
       </c>
       <c r="D81">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E81">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C82">
         <v>11</v>
       </c>
       <c r="D82">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E82">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C83">
         <v>12</v>
       </c>
       <c r="D83">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E83">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C84">
         <v>13</v>
       </c>
       <c r="D84">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E84">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C85">
         <v>14</v>
       </c>
       <c r="D85">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E85">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C86">
         <v>15</v>
       </c>
       <c r="D86">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E86">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C87">
         <v>16</v>
       </c>
       <c r="D87">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E87">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C88">
         <v>17</v>
       </c>
       <c r="D88">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E88">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C89">
         <v>18</v>
       </c>
       <c r="D89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E89">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C90">
         <v>19</v>
       </c>
       <c r="D90">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="E90">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C91">
         <v>20</v>
       </c>
       <c r="D91">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="E91">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C92">
         <v>21</v>
       </c>
       <c r="D92">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="E92">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C93">
         <v>22</v>
       </c>
       <c r="D93">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="E93">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C94">
         <v>23</v>
       </c>
       <c r="D94">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="E94">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C95">
         <v>24</v>
       </c>
       <c r="D95">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="E95">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C96">
         <v>25</v>
       </c>
       <c r="D96">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="E96">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C97">
         <v>26</v>
       </c>
       <c r="D97">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="E97">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>17</v>
       </c>
     </row>
-    <row r="98" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C98">
         <v>27</v>
       </c>
       <c r="D98">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="E98">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>17</v>
       </c>
     </row>
-    <row r="99" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C99">
         <v>28</v>
       </c>
       <c r="D99">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="E99">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C100">
         <v>29</v>
       </c>
       <c r="D100">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="E100">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C101">
         <v>30</v>
       </c>
       <c r="D101">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="E101">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>17</v>
       </c>
     </row>
-    <row r="102" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C102">
         <v>31</v>
       </c>
       <c r="D102">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="E102">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>17</v>
       </c>
     </row>
-    <row r="103" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C103">
         <v>32</v>
       </c>
       <c r="D103">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="E103">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
     </row>
-    <row r="104" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C104">
         <v>33</v>
       </c>
       <c r="D104">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="E104">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
     </row>
-    <row r="105" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C105">
         <v>34</v>
       </c>
       <c r="D105">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="E105">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
     </row>
-    <row r="106" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C106">
         <v>35</v>
       </c>
       <c r="D106">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="E106">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
     </row>
-    <row r="107" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C107">
         <v>36</v>
       </c>
       <c r="D107">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="E107">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
     </row>
-    <row r="108" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C108">
         <v>37</v>
       </c>
       <c r="D108">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="E108">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
     </row>
-    <row r="109" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C109">
         <v>38</v>
       </c>
       <c r="D109">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="E109">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
     </row>
-    <row r="110" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C110">
         <v>39</v>
       </c>
       <c r="D110">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="E110">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
     </row>
-    <row r="111" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C111">
         <v>40</v>
       </c>
       <c r="D111">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="E111">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
     </row>
-    <row r="112" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C112">
         <v>41</v>
       </c>
       <c r="D112">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="E112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
     </row>
-    <row r="113" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C113">
         <v>42</v>
       </c>
       <c r="D113">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="E113">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
     </row>
-    <row r="114" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C114">
         <v>43</v>
       </c>
       <c r="D114">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="E114">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
     </row>
-    <row r="115" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C115">
         <v>44</v>
       </c>
       <c r="D115">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="E115">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
     </row>
-    <row r="116" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C116">
         <v>45</v>
       </c>
       <c r="D116">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="E116">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C117">
         <v>46</v>
       </c>
       <c r="D117">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="E117">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C118">
         <v>47</v>
       </c>
       <c r="D118">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="E118">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C119">
         <v>48</v>
       </c>
       <c r="D119">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="E119">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C120">
         <v>49</v>
       </c>
       <c r="D120">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="E120">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C121">
         <v>50</v>
       </c>
       <c r="D121">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="E121">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C122">
         <v>51</v>
       </c>
       <c r="D122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="E122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C123">
         <v>52</v>
       </c>
       <c r="D123">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="E123">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C124">
         <v>53</v>
       </c>
       <c r="D124">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="E124">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C125">
         <v>54</v>
       </c>
       <c r="D125">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="E125">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C126">
         <v>55</v>
       </c>
       <c r="D126">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="E126">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C127">
         <v>56</v>
       </c>
       <c r="D127">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="E127">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C128">
         <v>57</v>
       </c>
       <c r="D128">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="E128">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C129">
         <v>58</v>
       </c>
       <c r="D129">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5</v>
       </c>
       <c r="E129">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>14</v>
       </c>
     </row>
-    <row r="130" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C130">
         <v>59</v>
       </c>
       <c r="D130">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5</v>
       </c>
       <c r="E130">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>14</v>
       </c>
     </row>
-    <row r="131" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C131">
         <v>60</v>
       </c>
       <c r="D131">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5</v>
       </c>
       <c r="E131">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>14</v>
       </c>
     </row>
-    <row r="132" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C132">
         <v>61</v>
       </c>
       <c r="D132">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5</v>
       </c>
       <c r="E132">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>14</v>
       </c>
     </row>
-    <row r="133" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C133">
         <v>62</v>
       </c>
       <c r="D133">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5</v>
       </c>
       <c r="E133">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>14</v>
       </c>
     </row>
-    <row r="134" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C134">
         <v>63</v>
       </c>
       <c r="D134">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5</v>
       </c>
       <c r="E134">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>14</v>
       </c>
     </row>
-    <row r="135" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C135">
         <v>64</v>
       </c>
       <c r="D135">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5</v>
       </c>
       <c r="E135">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>14</v>
       </c>
     </row>
-    <row r="136" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C136">
         <v>65</v>
       </c>
       <c r="D136">
-        <f t="shared" ref="D136:D199" si="15">FLOOR((20*C136+128)/256,1)</f>
+        <f t="shared" ref="D136:D199" si="16">FLOOR((20*C136+128)/256,1)</f>
         <v>5</v>
       </c>
       <c r="E136">
-        <f t="shared" ref="E136:E199" si="16">19-D136</f>
+        <f t="shared" ref="E136:E199" si="17">19-D136</f>
         <v>14</v>
       </c>
     </row>
-    <row r="137" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C137">
         <v>66</v>
       </c>
       <c r="D137">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="E137">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>14</v>
       </c>
     </row>
-    <row r="138" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C138">
         <v>67</v>
       </c>
       <c r="D138">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="E138">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>14</v>
       </c>
     </row>
-    <row r="139" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C139">
         <v>68</v>
       </c>
       <c r="D139">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="E139">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>14</v>
       </c>
     </row>
-    <row r="140" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C140">
         <v>69</v>
       </c>
       <c r="D140">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="E140">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>14</v>
       </c>
     </row>
-    <row r="141" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C141">
         <v>70</v>
       </c>
       <c r="D141">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="E141">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>14</v>
       </c>
     </row>
-    <row r="142" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C142">
         <v>71</v>
       </c>
       <c r="D142">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="E142">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
     </row>
-    <row r="143" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C143">
         <v>72</v>
       </c>
       <c r="D143">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="E143">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
     </row>
-    <row r="144" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C144">
         <v>73</v>
       </c>
       <c r="D144">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="E144">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
     </row>
-    <row r="145" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C145">
         <v>74</v>
       </c>
       <c r="D145">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="E145">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
     </row>
-    <row r="146" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C146">
         <v>75</v>
       </c>
       <c r="D146">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="E146">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C147">
         <v>76</v>
       </c>
       <c r="D147">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="E147">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
     </row>
-    <row r="148" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C148">
         <v>77</v>
       </c>
       <c r="D148">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="E148">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
     </row>
-    <row r="149" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C149">
         <v>78</v>
       </c>
       <c r="D149">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="E149">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
     </row>
-    <row r="150" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C150">
         <v>79</v>
       </c>
       <c r="D150">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="E150">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C151">
         <v>80</v>
       </c>
       <c r="D151">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="E151">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
     </row>
-    <row r="152" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C152">
         <v>81</v>
       </c>
       <c r="D152">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="E152">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
     </row>
-    <row r="153" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C153">
         <v>82</v>
       </c>
       <c r="D153">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="E153">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
     </row>
-    <row r="154" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C154">
         <v>83</v>
       </c>
       <c r="D154">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="E154">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
     </row>
-    <row r="155" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C155">
         <v>84</v>
       </c>
       <c r="D155">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="E155">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C156">
         <v>85</v>
       </c>
       <c r="D156">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="E156">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
-    <row r="157" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C157">
         <v>86</v>
       </c>
       <c r="D157">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="E157">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
-    <row r="158" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C158">
         <v>87</v>
       </c>
       <c r="D158">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="E158">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
-    <row r="159" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C159">
         <v>88</v>
       </c>
       <c r="D159">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="E159">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
-    <row r="160" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C160">
         <v>89</v>
       </c>
       <c r="D160">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="E160">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
-    <row r="161" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C161">
         <v>90</v>
       </c>
       <c r="D161">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="E161">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
-    <row r="162" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C162">
         <v>91</v>
       </c>
       <c r="D162">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="E162">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
-    <row r="163" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C163">
         <v>92</v>
       </c>
       <c r="D163">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="E163">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
-    <row r="164" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C164">
         <v>93</v>
       </c>
       <c r="D164">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="E164">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
-    <row r="165" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C165">
         <v>94</v>
       </c>
       <c r="D165">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="E165">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
-    <row r="166" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C166">
         <v>95</v>
       </c>
       <c r="D166">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="E166">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12</v>
       </c>
     </row>
-    <row r="167" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C167">
         <v>96</v>
       </c>
       <c r="D167">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="E167">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11</v>
       </c>
     </row>
-    <row r="168" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C168">
         <v>97</v>
       </c>
       <c r="D168">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="E168">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11</v>
       </c>
     </row>
-    <row r="169" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C169">
         <v>98</v>
       </c>
       <c r="D169">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="E169">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11</v>
       </c>
     </row>
-    <row r="170" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C170">
         <v>99</v>
       </c>
       <c r="D170">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="E170">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11</v>
       </c>
     </row>
-    <row r="171" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C171">
         <v>100</v>
       </c>
       <c r="D171">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="E171">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11</v>
       </c>
     </row>
-    <row r="172" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C172">
         <v>101</v>
       </c>
       <c r="D172">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="E172">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11</v>
       </c>
     </row>
-    <row r="173" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C173">
         <v>102</v>
       </c>
       <c r="D173">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="E173">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11</v>
       </c>
     </row>
-    <row r="174" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C174">
         <v>103</v>
       </c>
       <c r="D174">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="E174">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11</v>
       </c>
     </row>
-    <row r="175" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C175">
         <v>104</v>
       </c>
       <c r="D175">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="E175">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11</v>
       </c>
     </row>
-    <row r="176" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C176">
         <v>105</v>
       </c>
       <c r="D176">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="E176">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11</v>
       </c>
     </row>
-    <row r="177" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C177">
         <v>106</v>
       </c>
       <c r="D177">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="E177">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11</v>
       </c>
     </row>
-    <row r="178" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C178">
         <v>107</v>
       </c>
       <c r="D178">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="E178">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11</v>
       </c>
     </row>
-    <row r="179" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C179">
         <v>108</v>
       </c>
       <c r="D179">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="E179">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11</v>
       </c>
     </row>
-    <row r="180" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C180">
         <v>109</v>
       </c>
       <c r="D180">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>9</v>
       </c>
       <c r="E180">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="181" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C181">
+        <v>110</v>
+      </c>
+      <c r="D181">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="E181">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="182" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C182">
+        <v>111</v>
+      </c>
+      <c r="D182">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="E182">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="183" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C183">
+        <v>112</v>
+      </c>
+      <c r="D183">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="E183">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="184" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C184">
+        <v>113</v>
+      </c>
+      <c r="D184">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="E184">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="185" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C185">
+        <v>114</v>
+      </c>
+      <c r="D185">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="E185">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="186" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C186">
+        <v>115</v>
+      </c>
+      <c r="D186">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="E186">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="187" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C187">
+        <v>116</v>
+      </c>
+      <c r="D187">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="E187">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="188" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C188">
+        <v>117</v>
+      </c>
+      <c r="D188">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="E188">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="189" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C189">
+        <v>118</v>
+      </c>
+      <c r="D189">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="E189">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="190" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C190">
+        <v>119</v>
+      </c>
+      <c r="D190">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="E190">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="191" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C191">
+        <v>120</v>
+      </c>
+      <c r="D191">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="E191">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="192" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C192">
+        <v>121</v>
+      </c>
+      <c r="D192">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="E192">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="193" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C193">
+        <v>122</v>
+      </c>
+      <c r="D193">
         <f t="shared" si="16"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="181" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C181">
-        <v>110</v>
-      </c>
-      <c r="D181">
-        <f t="shared" si="15"/>
+      <c r="E193">
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
-      <c r="E181">
+    </row>
+    <row r="194" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C194">
+        <v>123</v>
+      </c>
+      <c r="D194">
         <f t="shared" si="16"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="182" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C182">
-        <v>111</v>
-      </c>
-      <c r="D182">
-        <f t="shared" si="15"/>
+      <c r="E194">
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
-      <c r="E182">
+    </row>
+    <row r="195" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C195">
+        <v>124</v>
+      </c>
+      <c r="D195">
         <f t="shared" si="16"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="183" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C183">
-        <v>112</v>
-      </c>
-      <c r="D183">
-        <f t="shared" si="15"/>
+      <c r="E195">
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
-      <c r="E183">
+    </row>
+    <row r="196" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C196">
+        <v>125</v>
+      </c>
+      <c r="D196">
         <f t="shared" si="16"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="184" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C184">
-        <v>113</v>
-      </c>
-      <c r="D184">
-        <f t="shared" si="15"/>
+      <c r="E196">
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
-      <c r="E184">
+    </row>
+    <row r="197" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C197">
+        <v>126</v>
+      </c>
+      <c r="D197">
         <f t="shared" si="16"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="185" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C185">
-        <v>114</v>
-      </c>
-      <c r="D185">
-        <f t="shared" si="15"/>
+      <c r="E197">
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
-      <c r="E185">
+    </row>
+    <row r="198" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C198">
+        <v>127</v>
+      </c>
+      <c r="D198">
         <f t="shared" si="16"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="186" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C186">
-        <v>115</v>
-      </c>
-      <c r="D186">
-        <f t="shared" si="15"/>
+      <c r="E198">
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
-      <c r="E186">
+    </row>
+    <row r="199" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C199">
+        <v>128</v>
+      </c>
+      <c r="D199">
         <f t="shared" si="16"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="187" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C187">
-        <v>116</v>
-      </c>
-      <c r="D187">
-        <f t="shared" si="15"/>
+      <c r="E199">
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
-      <c r="E187">
-        <f t="shared" si="16"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="188" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C188">
-        <v>117</v>
-      </c>
-      <c r="D188">
-        <f t="shared" si="15"/>
-        <v>9</v>
-      </c>
-      <c r="E188">
-        <f t="shared" si="16"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="189" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C189">
-        <v>118</v>
-      </c>
-      <c r="D189">
-        <f t="shared" si="15"/>
-        <v>9</v>
-      </c>
-      <c r="E189">
-        <f t="shared" si="16"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="190" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C190">
-        <v>119</v>
-      </c>
-      <c r="D190">
-        <f t="shared" si="15"/>
-        <v>9</v>
-      </c>
-      <c r="E190">
-        <f t="shared" si="16"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="191" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C191">
-        <v>120</v>
-      </c>
-      <c r="D191">
-        <f t="shared" si="15"/>
-        <v>9</v>
-      </c>
-      <c r="E191">
-        <f t="shared" si="16"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="192" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C192">
-        <v>121</v>
-      </c>
-      <c r="D192">
-        <f t="shared" si="15"/>
-        <v>9</v>
-      </c>
-      <c r="E192">
-        <f t="shared" si="16"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="193" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C193">
-        <v>122</v>
-      </c>
-      <c r="D193">
-        <f t="shared" si="15"/>
-        <v>10</v>
-      </c>
-      <c r="E193">
-        <f t="shared" si="16"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="194" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C194">
-        <v>123</v>
-      </c>
-      <c r="D194">
-        <f t="shared" si="15"/>
-        <v>10</v>
-      </c>
-      <c r="E194">
-        <f t="shared" si="16"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="195" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C195">
-        <v>124</v>
-      </c>
-      <c r="D195">
-        <f t="shared" si="15"/>
-        <v>10</v>
-      </c>
-      <c r="E195">
-        <f t="shared" si="16"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="196" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C196">
-        <v>125</v>
-      </c>
-      <c r="D196">
-        <f t="shared" si="15"/>
-        <v>10</v>
-      </c>
-      <c r="E196">
-        <f t="shared" si="16"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="197" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C197">
-        <v>126</v>
-      </c>
-      <c r="D197">
-        <f t="shared" si="15"/>
-        <v>10</v>
-      </c>
-      <c r="E197">
-        <f t="shared" si="16"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="198" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C198">
-        <v>127</v>
-      </c>
-      <c r="D198">
-        <f t="shared" si="15"/>
-        <v>10</v>
-      </c>
-      <c r="E198">
-        <f t="shared" si="16"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="199" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C199">
-        <v>128</v>
-      </c>
-      <c r="D199">
-        <f t="shared" si="15"/>
-        <v>10</v>
-      </c>
-      <c r="E199">
-        <f t="shared" si="16"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="200" spans="3:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="200" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C200">
         <v>129</v>
       </c>
       <c r="D200">
-        <f t="shared" ref="D200:D263" si="17">FLOOR((20*C200+128)/256,1)</f>
+        <f t="shared" ref="D200:D263" si="18">FLOOR((20*C200+128)/256,1)</f>
         <v>10</v>
       </c>
       <c r="E200">
-        <f t="shared" ref="E200:E263" si="18">19-D200</f>
+        <f t="shared" ref="E200:E263" si="19">19-D200</f>
         <v>9</v>
       </c>
     </row>
-    <row r="201" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C201">
         <v>130</v>
       </c>
       <c r="D201">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>10</v>
       </c>
       <c r="E201">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
     </row>
-    <row r="202" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C202">
         <v>131</v>
       </c>
       <c r="D202">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>10</v>
       </c>
       <c r="E202">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
     </row>
-    <row r="203" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C203">
         <v>132</v>
       </c>
       <c r="D203">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>10</v>
       </c>
       <c r="E203">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
     </row>
-    <row r="204" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C204">
         <v>133</v>
       </c>
       <c r="D204">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>10</v>
       </c>
       <c r="E204">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
     </row>
-    <row r="205" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C205">
         <v>134</v>
       </c>
       <c r="D205">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>10</v>
       </c>
       <c r="E205">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
     </row>
-    <row r="206" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C206">
         <v>135</v>
       </c>
       <c r="D206">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="E206">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
     </row>
-    <row r="207" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C207">
         <v>136</v>
       </c>
       <c r="D207">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="E207">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
     </row>
-    <row r="208" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C208">
         <v>137</v>
       </c>
       <c r="D208">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="E208">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
     </row>
-    <row r="209" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="209" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C209">
         <v>138</v>
       </c>
       <c r="D209">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="E209">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
     </row>
-    <row r="210" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="210" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C210">
         <v>139</v>
       </c>
       <c r="D210">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="E210">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
     </row>
-    <row r="211" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="211" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C211">
         <v>140</v>
       </c>
       <c r="D211">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="E211">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
     </row>
-    <row r="212" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="212" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C212">
         <v>141</v>
       </c>
       <c r="D212">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="E212">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
     </row>
-    <row r="213" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C213">
         <v>142</v>
       </c>
       <c r="D213">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="E213">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
     </row>
-    <row r="214" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C214">
         <v>143</v>
       </c>
       <c r="D214">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="E214">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
     </row>
-    <row r="215" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C215">
         <v>144</v>
       </c>
       <c r="D215">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="E215">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
     </row>
-    <row r="216" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C216">
         <v>145</v>
       </c>
       <c r="D216">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="E216">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
     </row>
-    <row r="217" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C217">
         <v>146</v>
       </c>
       <c r="D217">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="E217">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
     </row>
-    <row r="218" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C218">
         <v>147</v>
       </c>
       <c r="D218">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="E218">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
     </row>
-    <row r="219" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C219">
         <v>148</v>
       </c>
       <c r="D219">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="E219">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7</v>
       </c>
     </row>
-    <row r="220" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C220">
         <v>149</v>
       </c>
       <c r="D220">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="E220">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7</v>
       </c>
     </row>
-    <row r="221" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C221">
         <v>150</v>
       </c>
       <c r="D221">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="E221">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7</v>
       </c>
     </row>
-    <row r="222" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C222">
         <v>151</v>
       </c>
       <c r="D222">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="E222">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7</v>
       </c>
     </row>
-    <row r="223" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C223">
         <v>152</v>
       </c>
       <c r="D223">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="E223">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7</v>
       </c>
     </row>
-    <row r="224" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C224">
         <v>153</v>
       </c>
       <c r="D224">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="E224">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7</v>
       </c>
     </row>
-    <row r="225" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="225" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C225">
         <v>154</v>
       </c>
       <c r="D225">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="E225">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7</v>
       </c>
     </row>
-    <row r="226" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="226" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C226">
         <v>155</v>
       </c>
       <c r="D226">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="E226">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7</v>
       </c>
     </row>
-    <row r="227" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="227" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C227">
         <v>156</v>
       </c>
       <c r="D227">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="E227">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7</v>
       </c>
     </row>
-    <row r="228" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="228" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C228">
         <v>157</v>
       </c>
       <c r="D228">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="E228">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7</v>
       </c>
     </row>
-    <row r="229" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="229" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C229">
         <v>158</v>
       </c>
       <c r="D229">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="E229">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7</v>
       </c>
     </row>
-    <row r="230" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="230" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C230">
         <v>159</v>
       </c>
       <c r="D230">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="E230">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7</v>
       </c>
     </row>
-    <row r="231" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="231" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C231">
         <v>160</v>
       </c>
       <c r="D231">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="E231">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6</v>
       </c>
     </row>
-    <row r="232" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="232" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C232">
         <v>161</v>
       </c>
       <c r="D232">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="E232">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6</v>
       </c>
     </row>
-    <row r="233" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="233" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C233">
         <v>162</v>
       </c>
       <c r="D233">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="E233">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6</v>
       </c>
     </row>
-    <row r="234" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="234" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C234">
         <v>163</v>
       </c>
       <c r="D234">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="E234">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6</v>
       </c>
     </row>
-    <row r="235" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="235" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C235">
         <v>164</v>
       </c>
       <c r="D235">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="E235">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6</v>
       </c>
     </row>
-    <row r="236" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C236">
         <v>165</v>
       </c>
       <c r="D236">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="E236">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6</v>
       </c>
     </row>
-    <row r="237" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="237" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C237">
         <v>166</v>
       </c>
       <c r="D237">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="E237">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6</v>
       </c>
     </row>
-    <row r="238" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="238" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C238">
         <v>167</v>
       </c>
       <c r="D238">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="E238">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6</v>
       </c>
     </row>
-    <row r="239" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="239" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C239">
         <v>168</v>
       </c>
       <c r="D239">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="E239">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6</v>
       </c>
     </row>
-    <row r="240" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C240">
         <v>169</v>
       </c>
       <c r="D240">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="E240">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6</v>
       </c>
     </row>
-    <row r="241" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="241" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C241">
         <v>170</v>
       </c>
       <c r="D241">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="E241">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6</v>
       </c>
     </row>
-    <row r="242" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="242" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C242">
         <v>171</v>
       </c>
       <c r="D242">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="E242">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6</v>
       </c>
     </row>
-    <row r="243" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="243" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C243">
         <v>172</v>
       </c>
       <c r="D243">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="E243">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6</v>
       </c>
     </row>
-    <row r="244" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="244" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C244">
         <v>173</v>
       </c>
       <c r="D244">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="E244">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="245" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C245">
         <v>174</v>
       </c>
       <c r="D245">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="E245">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="246" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C246">
         <v>175</v>
       </c>
       <c r="D246">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="E246">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
     </row>
-    <row r="247" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="247" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C247">
         <v>176</v>
       </c>
       <c r="D247">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="E247">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
     </row>
-    <row r="248" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="248" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C248">
         <v>177</v>
       </c>
       <c r="D248">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="E248">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
     </row>
-    <row r="249" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="249" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C249">
         <v>178</v>
       </c>
       <c r="D249">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="E249">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
     </row>
-    <row r="250" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="250" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C250">
         <v>179</v>
       </c>
       <c r="D250">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="E250">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
     </row>
-    <row r="251" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="251" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C251">
         <v>180</v>
       </c>
       <c r="D251">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="E251">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
     </row>
-    <row r="252" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="252" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C252">
         <v>181</v>
       </c>
       <c r="D252">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="E252">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
     </row>
-    <row r="253" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="253" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C253">
         <v>182</v>
       </c>
       <c r="D253">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="E253">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
     </row>
-    <row r="254" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="254" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C254">
         <v>183</v>
       </c>
       <c r="D254">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="E254">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
     </row>
-    <row r="255" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="255" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C255">
         <v>184</v>
       </c>
       <c r="D255">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="E255">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
     </row>
-    <row r="256" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="256" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C256">
         <v>185</v>
       </c>
       <c r="D256">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="E256">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
     </row>
-    <row r="257" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="257" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C257">
         <v>186</v>
       </c>
       <c r="D257">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="E257">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
-    <row r="258" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="258" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C258">
         <v>187</v>
       </c>
       <c r="D258">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="E258">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
-    <row r="259" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="259" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C259">
         <v>188</v>
       </c>
       <c r="D259">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="E259">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
-    <row r="260" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="260" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C260">
         <v>189</v>
       </c>
       <c r="D260">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="E260">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
-    <row r="261" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="261" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C261">
         <v>190</v>
       </c>
       <c r="D261">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="E261">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
-    <row r="262" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="262" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C262">
         <v>191</v>
       </c>
       <c r="D262">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="E262">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
-    <row r="263" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="263" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C263">
         <v>192</v>
       </c>
       <c r="D263">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="E263">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
-    <row r="264" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="264" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C264">
         <v>193</v>
       </c>
       <c r="D264">
-        <f t="shared" ref="D264:D327" si="19">FLOOR((20*C264+128)/256,1)</f>
+        <f t="shared" ref="D264:D326" si="20">FLOOR((20*C264+128)/256,1)</f>
         <v>15</v>
       </c>
       <c r="E264">
-        <f t="shared" ref="E264:E327" si="20">19-D264</f>
+        <f t="shared" ref="E264:E326" si="21">19-D264</f>
         <v>4</v>
       </c>
     </row>
-    <row r="265" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="265" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C265">
         <v>194</v>
       </c>
       <c r="D265">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>15</v>
       </c>
       <c r="E265">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>4</v>
       </c>
     </row>
-    <row r="266" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="266" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C266">
         <v>195</v>
       </c>
       <c r="D266">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>15</v>
       </c>
       <c r="E266">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>4</v>
       </c>
     </row>
-    <row r="267" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="267" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C267">
         <v>196</v>
       </c>
       <c r="D267">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>15</v>
       </c>
       <c r="E267">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>4</v>
       </c>
     </row>
-    <row r="268" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="268" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C268">
         <v>197</v>
       </c>
       <c r="D268">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>15</v>
       </c>
       <c r="E268">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>4</v>
       </c>
     </row>
-    <row r="269" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="269" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C269">
         <v>198</v>
       </c>
       <c r="D269">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>15</v>
       </c>
       <c r="E269">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>4</v>
       </c>
     </row>
-    <row r="270" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="270" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C270">
         <v>199</v>
       </c>
       <c r="D270">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>16</v>
       </c>
       <c r="E270">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
     </row>
-    <row r="271" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="271" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C271">
         <v>200</v>
       </c>
       <c r="D271">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>16</v>
       </c>
       <c r="E271">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
     </row>
-    <row r="272" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="272" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C272">
         <v>201</v>
       </c>
       <c r="D272">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>16</v>
       </c>
       <c r="E272">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
     </row>
-    <row r="273" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="273" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C273">
         <v>202</v>
       </c>
       <c r="D273">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>16</v>
       </c>
       <c r="E273">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
     </row>
-    <row r="274" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="274" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C274">
         <v>203</v>
       </c>
       <c r="D274">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>16</v>
       </c>
       <c r="E274">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
     </row>
-    <row r="275" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="275" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C275">
         <v>204</v>
       </c>
       <c r="D275">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>16</v>
       </c>
       <c r="E275">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
     </row>
-    <row r="276" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="276" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C276">
         <v>205</v>
       </c>
       <c r="D276">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>16</v>
       </c>
       <c r="E276">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
     </row>
-    <row r="277" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="277" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C277">
         <v>206</v>
       </c>
       <c r="D277">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>16</v>
       </c>
       <c r="E277">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
     </row>
-    <row r="278" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="278" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C278">
         <v>207</v>
       </c>
       <c r="D278">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>16</v>
       </c>
       <c r="E278">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
     </row>
-    <row r="279" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="279" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C279">
         <v>208</v>
       </c>
       <c r="D279">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>16</v>
       </c>
       <c r="E279">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
     </row>
-    <row r="280" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="280" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C280">
         <v>209</v>
       </c>
       <c r="D280">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>16</v>
       </c>
       <c r="E280">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
     </row>
-    <row r="281" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="281" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C281">
         <v>210</v>
       </c>
       <c r="D281">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>16</v>
       </c>
       <c r="E281">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
     </row>
-    <row r="282" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="282" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C282">
         <v>211</v>
       </c>
       <c r="D282">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>16</v>
       </c>
       <c r="E282">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
     </row>
-    <row r="283" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="283" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C283">
         <v>212</v>
       </c>
       <c r="D283">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>17</v>
       </c>
       <c r="E283">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
     </row>
-    <row r="284" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="284" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C284">
         <v>213</v>
       </c>
       <c r="D284">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>17</v>
       </c>
       <c r="E284">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
     </row>
-    <row r="285" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="285" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C285">
         <v>214</v>
       </c>
       <c r="D285">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>17</v>
       </c>
       <c r="E285">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
     </row>
-    <row r="286" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="286" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C286">
         <v>215</v>
       </c>
       <c r="D286">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>17</v>
       </c>
       <c r="E286">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
     </row>
-    <row r="287" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="287" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C287">
         <v>216</v>
       </c>
       <c r="D287">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>17</v>
       </c>
       <c r="E287">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
     </row>
-    <row r="288" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="288" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C288">
         <v>217</v>
       </c>
       <c r="D288">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>17</v>
       </c>
       <c r="E288">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
     </row>
-    <row r="289" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="289" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C289">
         <v>218</v>
       </c>
       <c r="D289">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>17</v>
       </c>
       <c r="E289">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
     </row>
-    <row r="290" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="290" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C290">
         <v>219</v>
       </c>
       <c r="D290">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>17</v>
       </c>
       <c r="E290">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
     </row>
-    <row r="291" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="291" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C291">
         <v>220</v>
       </c>
       <c r="D291">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>17</v>
       </c>
       <c r="E291">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
     </row>
-    <row r="292" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="292" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C292">
         <v>221</v>
       </c>
       <c r="D292">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>17</v>
       </c>
       <c r="E292">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
     </row>
-    <row r="293" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="293" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C293">
         <v>222</v>
       </c>
       <c r="D293">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>17</v>
       </c>
       <c r="E293">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
     </row>
-    <row r="294" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="294" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C294">
         <v>223</v>
       </c>
       <c r="D294">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>17</v>
       </c>
       <c r="E294">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
     </row>
-    <row r="295" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="295" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C295">
         <v>224</v>
       </c>
       <c r="D295">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>18</v>
       </c>
       <c r="E295">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="296" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C296">
         <v>225</v>
       </c>
       <c r="D296">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>18</v>
       </c>
       <c r="E296">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="297" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C297">
         <v>226</v>
       </c>
       <c r="D297">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>18</v>
       </c>
       <c r="E297">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="298" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C298">
         <v>227</v>
       </c>
       <c r="D298">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>18</v>
       </c>
       <c r="E298">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="299" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C299">
         <v>228</v>
       </c>
       <c r="D299">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>18</v>
       </c>
       <c r="E299">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="300" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C300">
         <v>229</v>
       </c>
       <c r="D300">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>18</v>
       </c>
       <c r="E300">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="301" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C301">
         <v>230</v>
       </c>
       <c r="D301">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>18</v>
       </c>
       <c r="E301">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="302" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C302">
         <v>231</v>
       </c>
       <c r="D302">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>18</v>
       </c>
       <c r="E302">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="303" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C303">
         <v>232</v>
       </c>
       <c r="D303">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>18</v>
       </c>
       <c r="E303">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="304" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C304">
         <v>233</v>
       </c>
       <c r="D304">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>18</v>
       </c>
       <c r="E304">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="305" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C305">
         <v>234</v>
       </c>
       <c r="D305">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>18</v>
       </c>
       <c r="E305">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="306" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C306">
         <v>235</v>
       </c>
       <c r="D306">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>18</v>
       </c>
       <c r="E306">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="307" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C307">
         <v>236</v>
       </c>
       <c r="D307">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>18</v>
       </c>
       <c r="E307">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="308" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C308">
         <v>237</v>
       </c>
       <c r="D308">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>19</v>
       </c>
       <c r="E308">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="309" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C309">
         <v>238</v>
       </c>
       <c r="D309">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>19</v>
       </c>
       <c r="E309">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="310" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C310">
         <v>239</v>
       </c>
       <c r="D310">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>19</v>
       </c>
       <c r="E310">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="311" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C311">
         <v>240</v>
       </c>
       <c r="D311">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>19</v>
       </c>
       <c r="E311">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="312" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C312">
         <v>241</v>
       </c>
       <c r="D312">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>19</v>
       </c>
       <c r="E312">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="313" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C313">
         <v>242</v>
       </c>
       <c r="D313">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>19</v>
       </c>
       <c r="E313">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="314" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C314">
         <v>243</v>
       </c>
       <c r="D314">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>19</v>
       </c>
       <c r="E314">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="315" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C315">
         <v>244</v>
       </c>
       <c r="D315">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>19</v>
       </c>
       <c r="E315">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="316" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C316">
         <v>245</v>
       </c>
       <c r="D316">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>19</v>
       </c>
       <c r="E316">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="317" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C317">
         <v>246</v>
       </c>
       <c r="D317">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>19</v>
       </c>
       <c r="E317">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="318" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C318">
         <v>247</v>
       </c>
       <c r="D318">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>19</v>
       </c>
       <c r="E318">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="319" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C319">
         <v>248</v>
       </c>
       <c r="D319">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>19</v>
       </c>
       <c r="E319">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="320" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C320">
         <v>249</v>
       </c>
       <c r="D320">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>19</v>
       </c>
       <c r="E320">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="321" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C321">
         <v>250</v>
       </c>
       <c r="D321">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>20</v>
       </c>
       <c r="E321">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="322" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="322" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C322">
         <v>251</v>
       </c>
       <c r="D322">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>20</v>
       </c>
       <c r="E322">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="323" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="323" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C323">
         <v>252</v>
       </c>
       <c r="D323">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>20</v>
       </c>
       <c r="E323">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="324" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="324" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C324">
         <v>253</v>
       </c>
       <c r="D324">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>20</v>
       </c>
       <c r="E324">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="325" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="325" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C325">
         <v>254</v>
       </c>
       <c r="D325">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>20</v>
       </c>
       <c r="E325">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="326" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="326" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C326">
         <v>255</v>
       </c>
       <c r="D326">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>20</v>
       </c>
       <c r="E326">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>-1</v>
       </c>
     </row>

</xml_diff>